<commit_message>
Updated data retrieval with attempts to capture the base form of searched for phrases and their plurals. Implemented some unit Tests to this end.
</commit_message>
<xml_diff>
--- a/perf_results.xlsx
+++ b/perf_results.xlsx
@@ -472,16 +472,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3.877142667770386</v>
+        <v>5.133420467376709</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01011562347412109</v>
+        <v>0.01023483276367188</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5746762752532959</v>
+        <v>0.6066503524780273</v>
       </c>
       <c r="E2" t="n">
-        <v>4.489103555679321</v>
+        <v>5.788755893707275</v>
       </c>
       <c r="F2" t="n">
         <v>200</v>
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2003965377807617</v>
+        <v>0.2404730319976807</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -503,7 +503,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2003965377807617</v>
+        <v>0.2404730319976807</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -516,19 +516,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>27.8476459980011</v>
+        <v>52.86789798736572</v>
       </c>
       <c r="C4" t="n">
-        <v>0.07632088661193848</v>
+        <v>0.07901811599731445</v>
       </c>
       <c r="D4" t="n">
-        <v>5.676680088043213</v>
+        <v>5.585498094558716</v>
       </c>
       <c r="E4" t="n">
-        <v>33.86032843589783</v>
+        <v>58.88949418067932</v>
       </c>
       <c r="F4" t="n">
-        <v>1537</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="5">
@@ -538,16 +538,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17.65989542007446</v>
+        <v>33.35113787651062</v>
       </c>
       <c r="C5" t="n">
-        <v>0.01912832260131836</v>
+        <v>0.02010226249694824</v>
       </c>
       <c r="D5" t="n">
-        <v>1.046591281890869</v>
+        <v>1.087490320205688</v>
       </c>
       <c r="E5" t="n">
-        <v>18.77896952629089</v>
+        <v>34.52986168861389</v>
       </c>
       <c r="F5" t="n">
         <v>379</v>
@@ -560,16 +560,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>25.48498320579529</v>
+        <v>47.25594401359558</v>
       </c>
       <c r="C6" t="n">
-        <v>0.07573127746582031</v>
+        <v>0.07221770286560059</v>
       </c>
       <c r="D6" t="n">
-        <v>4.533211231231689</v>
+        <v>4.555901527404785</v>
       </c>
       <c r="E6" t="n">
-        <v>30.30722856521606</v>
+        <v>52.17206954956055</v>
       </c>
       <c r="F6" t="n">
         <v>1234</v>
@@ -582,16 +582,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1882679462432861</v>
+        <v>0.1918485164642334</v>
       </c>
       <c r="C7" t="n">
-        <v>0.001001119613647461</v>
+        <v>0.00099945068359375</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1892690658569336</v>
+        <v>0.1928479671478271</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -604,7 +604,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1889655590057373</v>
+        <v>0.199887752532959</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -613,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1889655590057373</v>
+        <v>0.199887752532959</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>

</xml_diff>